<commit_message>
changed strip for split
</commit_message>
<xml_diff>
--- a/output/nz_sectorial.xlsx
+++ b/output/nz_sectorial.xlsx
@@ -7,23 +7,26 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="C" sheetId="1" r:id="rId1"/>
-    <sheet name="F" sheetId="2" r:id="rId2"/>
-    <sheet name="A" sheetId="3" r:id="rId3"/>
-    <sheet name="M" sheetId="4" r:id="rId4"/>
-    <sheet name="R" sheetId="5" r:id="rId5"/>
+    <sheet name="Construction" sheetId="1" r:id="rId1"/>
+    <sheet name="Financial" sheetId="2" r:id="rId2"/>
+    <sheet name="Agriculture" sheetId="3" r:id="rId3"/>
+    <sheet name="Manufacturing" sheetId="4" r:id="rId4"/>
+    <sheet name="Rental," sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
     <t>Synthetic Control</t>
   </si>
   <si>
     <t>Canterbury</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -381,201 +384,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B2">
         <v>0.04906493091726361</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.04691903419910123</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B3">
         <v>0.04680049829108091</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.04668696534725243</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B4">
         <v>0.04788282528847553</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.04817567567567568</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B5">
         <v>0.05135211089803166</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.05033557046979865</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B6">
         <v>0.05344883329314909</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.05379746835443038</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B7">
         <v>0.06205063507048036</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.06148572652777034</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B8">
         <v>0.05781022893334799</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.05970452353150226</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B9">
         <v>0.06134013992483248</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.06115056479672084</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B10">
         <v>0.06393365867846391</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.06523373579231348</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B11">
         <v>0.06186301710861096</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.0607488647073944</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B12">
         <v>0.06189934540876829</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.05813177648040033</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B13">
         <v>0.05842649173065316</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.05822814955941891</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B14">
         <v>0.05477006248634197</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.06914873572747485</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B15">
         <v>0.0573063838588671</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.08298755186721991</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B16">
         <v>0.05523031418547152</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.08872620790629575</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B17">
         <v>0.05760304127226024</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>0.0983616769451193</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B18">
         <v>0.05944625856069585</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>0.09969214052879391</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B19">
         <v>0.06178806729412574</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0.09143342311746105</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B20">
         <v>0.06530514786664837</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>0.08983619068385619</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21">
         <v>0.06792619332690435</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>0.08674308692586886</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B22">
         <v>0.07363023906146304</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>0.08592227020357804</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B23">
         <v>0.07586588963469139</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>0.08672113641443366</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B24">
         <v>0.07243658799368426</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>0.08358154657693095</v>
       </c>
     </row>
@@ -586,201 +661,273 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B2">
         <v>0.03007909689917373</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.02825805468809506</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B3">
         <v>0.0312470584851104</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.0283456575322604</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B4">
         <v>0.03227133885523309</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.03060810810810811</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B5">
         <v>0.03368547418708807</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.03362036216284665</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B6">
         <v>0.03596181342148747</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.03656821378340366</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B7">
         <v>0.03600914734951761</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.03840179958223984</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B8">
         <v>0.03567700225848598</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.03690917398588617</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B9">
         <v>0.03399763532083194</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.03512701968447643</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B10">
         <v>0.0324154514168459</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.03312546990402901</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B11">
         <v>0.03620547753348185</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.03654356953131694</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B12">
         <v>0.04322070504686332</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.04065888240200167</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B13">
         <v>0.03682373619835875</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.03433357148527427</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B14">
         <v>0.03832026340542466</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.02999585484417983</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B15">
         <v>0.03838882914442005</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.03146310662096338</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B16">
         <v>0.03944901694884345</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.03237351553603384</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B17">
         <v>0.04176885608579241</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>0.0328599015760294</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B18">
         <v>0.03945349891239387</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>0.02716407098877218</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B19">
         <v>0.03945074305864764</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0.02415388218760979</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B20">
         <v>0.0423302343339982</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>0.03109923955408978</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21">
         <v>0.04140153622595918</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>0.03459801028801211</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B22">
         <v>0.03977741698710291</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>0.03195558297347317</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B23">
         <v>0.0416315451951683</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>0.0338738917724191</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B24">
         <v>0.04201457510449433</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>0.0366976649007526</v>
       </c>
     </row>
@@ -791,201 +938,273 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B2">
         <v>0.05359692633657856</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.05567826947977759</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B3">
         <v>0.06871105031612298</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.07133536320139192</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B4">
         <v>0.07211490572690711</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.07290540540540541</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B5">
         <v>0.05364865705733975</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.05628719767000127</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B6">
         <v>0.05745812316334539</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.05291842475386779</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B7">
         <v>0.0530040633830141</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.04997054255262171</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B8">
         <v>0.04579997639083225</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.04046301467228512</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B9">
         <v>0.04696164018481796</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.04451646727991992</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B10">
         <v>0.05644971522673934</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.06364159037636549</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B11">
         <v>0.04595653451965806</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.05098106417616314</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B12">
         <v>0.0526401295090982</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.06609674728940784</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B13">
         <v>0.05954617393470901</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.07402556164166071</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B14">
         <v>0.05892382135152351</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.07306779213927724</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B15">
         <v>0.05018241983358682</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.06126646220458236</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B16">
         <v>0.06607430397563742</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.0816658532617537</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B17">
         <v>0.04555791321242324</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>0.04656450507693266</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B18">
         <v>0.04139462578682167</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>0.04122902330073645</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B19">
         <v>0.05119160630181905</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0.06118983487527813</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B20">
         <v>0.05356419995195776</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>0.06604159284799259</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21">
         <v>0.05000984983500588</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>0.06334699845940936</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B22">
         <v>0.05169042225300324</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>0.06706971005552129</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B23">
         <v>0.05166327670416251</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>0.07147291827054411</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B24">
         <v>0.05259850295154217</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>0.07416839089606876</v>
       </c>
     </row>
@@ -996,201 +1215,273 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B2">
         <v>0.1553477882710759</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.1668063066494021</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B3">
         <v>0.1553727857390066</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.1610120342177759</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B4">
         <v>0.1511350973436875</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.1587162162162162</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B5">
         <v>0.1523813399375723</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.1627833354438394</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B6">
         <v>0.1405091861772285</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.1557665260196906</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B7">
         <v>0.137163740578218</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.1533394033527931</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B8">
         <v>0.1338522087339745</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.1514951515459207</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B9">
         <v>0.1286596632894792</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.1400791192030885</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B10">
         <v>0.1245705057268068</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.130865507938614</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B11">
         <v>0.119025021170035</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.1364921600548368</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B12">
         <v>0.108952311036013</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.1265638031693078</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B13">
         <v>0.1096749628216678</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.1252282289433992</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B14">
         <v>0.1096089221402403</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.1224705128688247</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B15">
         <v>0.1055224540561837</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.1170485296770702</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B16">
         <v>0.1008952287409682</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.1063282902228729</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B17">
         <v>0.1074069403621688</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>0.1158661932349094</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B18">
         <v>0.1092625941465573</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>0.1238379814077025</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B19">
         <v>0.1005533435973455</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0.1099074833118632</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B20">
         <v>0.1004099791250133</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>0.1114230423287634</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21">
         <v>0.09698982205074165</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>0.1071624409222655</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B22">
         <v>0.09398303729603927</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>0.1078346699568168</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B23">
         <v>0.09027881262199755</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>0.1038567561526808</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B24">
         <v>0.08756269844834699</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>0.09338123280507492</v>
       </c>
     </row>
@@ -1201,201 +1492,273 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B2">
         <v>0.05624227328587624</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.05423109147688324</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B3">
         <v>0.05566408424711579</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.05437146585471944</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B4">
         <v>0.05468798672102409</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.05506756756756757</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B5">
         <v>0.05799484001456742</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.05774344687856148</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B6">
         <v>0.06012111909265384</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.0603609939052977</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B7">
         <v>0.0619137691866244</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.06121793155160409</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B8">
         <v>0.06374636810580475</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.06655835914098594</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B9">
         <v>0.06517340419509993</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.06748963347790858</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B10">
         <v>0.06151226160726138</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.05970545309804962</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B11">
         <v>0.06662331567342743</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.06383343329620426</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B12">
         <v>0.07230366247980437</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.07043369474562135</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B13">
         <v>0.07036640374229255</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.06961975073430182</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B14">
         <v>0.07192092760208396</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.07144741304593587</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B15">
         <v>0.07257663559556451</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.07007035901136568</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B16">
         <v>0.07090139809651759</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.07216528387831463</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B17">
         <v>0.06971867106598115</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>0.07020494611599078</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B18">
         <v>0.07104238262968995</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>0.06818181818181818</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B19">
         <v>0.07259247428125223</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0.06994378732872701</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B20">
         <v>0.06920275270034486</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>0.06609610509962113</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B21">
         <v>0.07141851010298812</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>0.06825599916442542</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B22">
         <v>0.07328085368004435</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>0.06679827267119062</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B23">
         <v>0.07593712762465718</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>0.06777261777634291</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B24">
         <v>0.07333224976142672</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>0.06643777995043314</v>
       </c>
     </row>

</xml_diff>